<commit_message>
import data from json
</commit_message>
<xml_diff>
--- a/public/benchmark_linguistics.xlsx
+++ b/public/benchmark_linguistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javier/Desktop/tmp/psycholinguistics_benchmark/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D356CA05-A1D4-2643-ADFE-1F5C6541145F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0DB0F7-7F70-BF40-83E8-5F8E6BCA4D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,11 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +485,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +520,7 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">

</xml_diff>